<commit_message>
Feature/reset-passord and ui my-ticket page, profile page
</commit_message>
<xml_diff>
--- a/MoTaCongViec.xlsx
+++ b/MoTaCongViec.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>STT</t>
   </si>
@@ -67,6 +67,13 @@
 2. Nộp sơ đồ CSDL mức quan niệm ERD
 3. Coding, Đưa source lên GIT, gửi link github
 4. Nộp phân công công việc nhóm</t>
+  </si>
+  <si>
+    <t>1. Hoàn thành mô hình dữ liệu mức ý niệm (ERD) thể hiện các thực thể và mối quan hệ chính của hệ thống bán vé sự kiện, bao gồm Người dùng, Sự kiện, Vé, Đơn hàng và Phân quyền người dùng.
+2. Hoàn thiện Use Case Đăng ký, Đăng nhập và Quản lý thông tin cá nhân, mô tả đầy đủ các bước tương tác giữa người dùng và hệ thống. Đảm bảo các Use Case thể hiện rõ phạm vi chức năng, luồng hoạt động và mối liên kết giữa người dùng với hệ thống.
+3. Thiết kế và xây dựng giao diện người dùng cho các màn hình đăng ký, đăng nhập và quản lý thông tin cá nhân, đảm bảo bố cục hợp lý, dễ sử dụng và đồng nhất phong cách. Hoàn thiện các chức năng cơ bản cho phép người dùng đăng ký tài khoản, đăng nhập hệ thống, chỉnh sửa và lưu thông tin cá nhân. Thực hiện phân quyền người dùng, đảm bảo mỗi nhóm đối tượng chỉ truy cập được vào các chức năng phù hợp.
+Kết quả đạt được:
+- Hoàn thành toàn bộ Use Case và giao diện liên quan đến đăng ký, đăng nhập và quản lý thông tin cá nhân, đáp ứng đúng yêu cầu trong phạm vi công việc tuần này, là nền tảng để phát triển các chức năng nâng cao trong những tuần tiếp theo như tạo sự kiện, mua vé và quản lý đơn hàng.</t>
   </si>
   <si>
     <t>Gặp offline tại trường vào sáng T7</t>
@@ -801,10 +808,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1133,8 +1140,8 @@
   <sheetPr/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1180,19 +1187,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="68" spans="1:5">
+    <row r="3" ht="303" spans="1:5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="51" spans="1:5">
@@ -1200,10 +1209,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
         <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
@@ -1215,10 +1224,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
@@ -1230,14 +1239,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="51" spans="1:5">
@@ -1245,10 +1254,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
@@ -1260,10 +1269,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
@@ -1275,14 +1284,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" ht="68" spans="1:5">
@@ -1290,10 +1299,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
@@ -1305,10 +1314,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
@@ -1320,14 +1329,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" ht="68" spans="1:5">
@@ -1335,14 +1344,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" ht="68" spans="1:5">
@@ -1350,14 +1359,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" ht="68" spans="1:5">
@@ -1365,14 +1374,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1380,14 +1389,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update UI and document
</commit_message>
<xml_diff>
--- a/MoTaCongViec.xlsx
+++ b/MoTaCongViec.xlsx
@@ -70,10 +70,10 @@
   </si>
   <si>
     <t>1. Hoàn thành mô hình dữ liệu mức ý niệm (ERD) thể hiện các thực thể và mối quan hệ chính của hệ thống bán vé sự kiện, bao gồm Người dùng, Sự kiện, Vé, Đơn hàng và Phân quyền người dùng.
-2. Hoàn thiện Use Case Đăng ký, Đăng nhập và Quản lý thông tin cá nhân, mô tả đầy đủ các bước tương tác giữa người dùng và hệ thống. Đảm bảo các Use Case thể hiện rõ phạm vi chức năng, luồng hoạt động và mối liên kết giữa người dùng với hệ thống.
-3. Thiết kế và xây dựng giao diện người dùng cho các màn hình đăng ký, đăng nhập và quản lý thông tin cá nhân, đảm bảo bố cục hợp lý, dễ sử dụng và đồng nhất phong cách. Hoàn thiện các chức năng cơ bản cho phép người dùng đăng ký tài khoản, đăng nhập hệ thống, chỉnh sửa và lưu thông tin cá nhân. Thực hiện phân quyền người dùng, đảm bảo mỗi nhóm đối tượng chỉ truy cập được vào các chức năng phù hợp.
-Kết quả đạt được:
-- Hoàn thành toàn bộ Use Case và giao diện liên quan đến đăng ký, đăng nhập và quản lý thông tin cá nhân, đáp ứng đúng yêu cầu trong phạm vi công việc tuần này, là nền tảng để phát triển các chức năng nâng cao trong những tuần tiếp theo như tạo sự kiện, mua vé và quản lý đơn hàng.</t>
+2. Thiết kế các use case cho phần quản lý thông tin cá nhân, đăng ký và đăng nhập để mô tả các chức năng chính của hệ thống.
+3. Xây dựng chức năng đăng ký, đăng nhập, quên mật khẩu và xác thực email, giúp người dùng có thể tạo tài khoản và lấy lại mật khẩu khi cần.
+4. Vẽ sơ đồ tuần tự cho các chức năng đăng ký, đăng nhập và quên mật khẩu để mô tả lại quá trình xử lý của hệ thống.
+5. Cài đặt cơ chế JWT và phân quyền người dùng, đảm bảo chỉ những người có quyền mới được truy cập vào các trang quản trị hoặc chức năng quan trọng.</t>
   </si>
   <si>
     <t>Gặp offline tại trường vào sáng T7</t>
@@ -1140,8 +1140,8 @@
   <sheetPr/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="303" spans="1:5">
+    <row r="3" ht="252" spans="1:5">
       <c r="A3" s="4">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update Frontend , Refactor code, Add Sequence Diagram and Activity Diagram
</commit_message>
<xml_diff>
--- a/MoTaCongViec.xlsx
+++ b/MoTaCongViec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29400" windowHeight="14000"/>
+    <workbookView windowWidth="29400" windowHeight="13420"/>
   </bookViews>
   <sheets>
     <sheet name="Mô tả công việc" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -85,6 +85,12 @@
     <t>1. Nộp mô tả use case
 2. Coding, cập nhật souce mới lên github
 3. Nộp phân công công việc nhóm</t>
+  </si>
+  <si>
+    <t>1. Chỉnh sửa lại mô hình dữ liệu mức ý niệm, thể hiện rõ các thực thể và mối quan hệ trong hệ thống bán vé sự kiện, đảm bảo tính logic và phù hợp với quy trình nghiệp vụ.
+2.  Hoàn thiện các sơ đồ tuần tự cho các chức năng.
+3. Hoàn thiện các sơ đồ hoạt động cho các chức năng.
+4.  Tiếp tục phát triền giao diện FrontEnd và refactor lại code dự án.</t>
   </si>
   <si>
     <t>09/11/2025</t>
@@ -787,7 +793,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,6 +815,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1141,7 +1150,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1166,7 +1175,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1204,17 +1213,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="51" spans="1:5">
+    <row r="4" ht="152" spans="1:5">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1223,11 +1234,11 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>15</v>
+      <c r="B5" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
@@ -1239,10 +1250,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
@@ -1254,10 +1265,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
@@ -1269,10 +1280,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
@@ -1283,11 +1294,11 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>21</v>
+      <c r="B9" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
@@ -1299,10 +1310,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
@@ -1313,11 +1324,11 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
@@ -1328,11 +1339,11 @@
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>25</v>
+      <c r="B12" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
@@ -1343,11 +1354,11 @@
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>26</v>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
@@ -1358,11 +1369,11 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>27</v>
+      <c r="B14" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
@@ -1373,11 +1384,11 @@
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>28</v>
+      <c r="B15" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
@@ -1388,11 +1399,11 @@
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>29</v>
+      <c r="B16" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">

</xml_diff>